<commit_message>
added generate pdf functionality
</commit_message>
<xml_diff>
--- a/house_expenses_data/house_expenses.xlsx
+++ b/house_expenses_data/house_expenses.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,138 +473,963 @@
           <t>Receipt_Reference</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45809</v>
+        <v>45570</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Foundation</t>
+          <t>House Plot</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Concrete</t>
+          <t>Land Registration</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Initial foundation concrete work</t>
+          <t>Land registration fees</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>FOUND001</t>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>registration for the land</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45809</v>
+        <v>45570</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Permits</t>
+          <t>House Plot</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Building Permit</t>
+          <t>Land Cost</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Building permit application fee</t>
+          <t>Land purchase</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2500</v>
+        <v>2500000</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Credit Card</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>PERM001</t>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>cost for the land</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45809</v>
+        <v>45721</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Foundation</t>
+          <t>Planning</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Concrete</t>
+          <t>House Plan</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Initial foundation concrete work</t>
+          <t>House plan design</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>15000</v>
+        <v>3500</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Bank Transfer</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>FOUND001</t>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>plan design by zara</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
+        <v>45736</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Building Plan Approval</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>EC market value</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>EC approval</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>700</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>sub-register office</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45738</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Building Material</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Material (Wood)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Teak wood purchase</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>701000</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>bought teak</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45748</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Other Expenses</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Poojari fees</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>500</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Given to Poojari</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45748</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Personal Transport</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Travel expenses</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>500</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>General transportation to pormamilla</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45748</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Teak transportation</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>transportation of teak to home</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45748</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Coolie (Wood)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Labor charges for teak</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Coolie charges for teak</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45748</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Permits</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Check post fees</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>600</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>check post cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45748</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Permits</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Transportation permit</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>2600</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Permit for transportation of teak</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45756</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Doors &amp; Windows</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Carpenter</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Carpenter advance</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Advance for Aachari</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45760</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Coolie</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Construction labor advance</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Advance for the Coolie, construction</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45768</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Building Plan Approval</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Property Tax</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Property tax payment</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>8197</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>property tax</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45770</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Initial Setup</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Basic Things</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Utility connections</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Electrical &amp; water connections</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45773</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Pooja</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Bhumi Pooja</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Pooja items</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>1530</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>vastralu</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45773</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Building Material</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>RR Stones</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Stone purchase</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>4000</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>1 tractor</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45773</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Initial Setup</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Construction Equipment</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Construction tools</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>2700</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>bought 10 tubs, 2 paralu</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45775</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Coolie</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>First payment after marking</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>first payment to masthan, after marking</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45775</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Pooja</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Bhumi Pooja</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Pooja materials</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Bought things for Bhumi Pooja</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>45776</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Ramapuram Kankara</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Kankara before Bhumi Pooja</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>23200</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>6 units kankara before bhumi pooja</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>45778</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>kankara</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Kankara stones</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>4800</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1 tractor 40mm kankara</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>45783</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>JCB</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>JCB work</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>16000</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>rent for JCB</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>45798</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Bricks</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Brick purchase</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Not specified</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>fly ash bricks</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>45806</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Iron</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Iron payment</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>75000</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>PhonePe</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Iron ; phonepe</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45806</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Cement</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Cement payment</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>20000</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>PhonePe</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>cement; Phonepe</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
         <v>45809</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
         <is>
           <t>Permits</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Building Permit</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Building permit application fee</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="E28" t="n">
         <v>2500</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>Credit Card</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>PERM001</t>
         </is>
       </c>
+      <c r="H28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>45809</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Construction</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Labour charges</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Initial foundation concrete work</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>15000</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Bank Transfer</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>FOUND001</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>